<commit_message>
Update du journal de travail
J'ai compléter les dernières informations sur le journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/JournauxMarcosDMS.xlsx
+++ b/Documentation/JournauxMarcosDMS.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -193,6 +193,24 @@
   </si>
   <si>
     <t>Dernière mise a jour du cahier des charges.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Préparation des questions </t>
+  </si>
+  <si>
+    <t>On a cherché plusieurs question a poser au client durant le rendez-vous</t>
+  </si>
+  <si>
+    <t>Imprimer</t>
+  </si>
+  <si>
+    <t>J'ai imprimer les documents pour préparer notre rendez-vous</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>Envoie du mail aux clients pour le rendez-vous</t>
   </si>
 </sst>
 </file>
@@ -743,13 +761,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -775,36 +823,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1411,7 +1429,7 @@
   <dimension ref="B1:N9999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1433,27 +1451,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1461,14 +1479,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="39" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="50"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1495,14 +1513,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="37" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="48"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1530,14 +1548,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="35">
+      <c r="C6" s="39"/>
+      <c r="D6" s="45">
         <v>44957</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="46"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1565,15 +1583,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49">
+      <c r="C7" s="37"/>
+      <c r="D7" s="40">
         <f>SUM(Tableau1[Durée])</f>
-        <v>0.28958333333333319</v>
+        <v>0.31319444444444422</v>
       </c>
-      <c r="E7" s="50"/>
+      <c r="E7" s="41"/>
       <c r="G7" s="4">
         <v>44927</v>
       </c>
@@ -1629,10 +1647,10 @@
     </row>
     <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="42"/>
+      <c r="D9" s="31"/>
       <c r="G9" s="4">
         <v>44927</v>
       </c>
@@ -1663,10 +1681,10 @@
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="44"/>
+      <c r="D10" s="33"/>
       <c r="G10" s="4">
         <v>44927</v>
       </c>
@@ -1697,10 +1715,10 @@
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="46"/>
+      <c r="D11" s="35"/>
       <c r="G11" s="4">
         <v>44927</v>
       </c>
@@ -1943,44 +1961,86 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G20" s="4"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
+    <row r="20" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G20" s="4">
+        <v>44966</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.65277777777777779</v>
+      </c>
       <c r="J20" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>1.388888888888884E-2</v>
       </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-    </row>
-    <row r="21" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
+      <c r="K20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G21" s="4">
+        <v>44966</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.65347222222222223</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.65625</v>
+      </c>
       <c r="J21" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>2.7777777777777679E-3</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="K21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="22" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
+      <c r="G22" s="4">
+        <v>44966</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="J22" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
+        <v>6.9444444444444198E-3</v>
       </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
+      <c r="K22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="23" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G23" s="4"/>
@@ -44385,18 +44445,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:N2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G1:N2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -44757,12 +44817,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -44936,15 +44993,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -44968,17 +45036,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise a jour de mon journal de travail ainsi que le journal de bord
J'ai mis a jour mon journal de travail pour les activités effectuer hier et modifier pour les activité effectué aujourd'hui. J'ai modifié mon journal de bord vu que nous avons reçu un feedback du maitre du projet.
</commit_message>
<xml_diff>
--- a/Documentation/JournauxMarcosDMS.xlsx
+++ b/Documentation/JournauxMarcosDMS.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Journal De Travail" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil3" sheetId="4" r:id="rId2"/>
+    <sheet name="Journal de bord" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -199,6 +199,33 @@
   </si>
   <si>
     <t>On a attendu Monsieur Meylan</t>
+  </si>
+  <si>
+    <t>IceScrum</t>
+  </si>
+  <si>
+    <t>Mise à jour du IceScrum (Ajout de tache dans les sprints.)</t>
+  </si>
+  <si>
+    <t>Mettre les dernières taches a jour dans le IceScrum ainsi que ajouter les dernières taches dans les sprints</t>
+  </si>
+  <si>
+    <t>Cahier des charges</t>
+  </si>
+  <si>
+    <t>Modification du cahier des charges par rapport aux dire du prof</t>
+  </si>
+  <si>
+    <t>Dossier de projet</t>
+  </si>
+  <si>
+    <t>Modification du dossier de projet par rapport aux dire du prof</t>
+  </si>
+  <si>
+    <t>Monsieur Meylan</t>
+  </si>
+  <si>
+    <t>Feedback du cahier des charges</t>
   </si>
 </sst>
 </file>
@@ -668,7 +695,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -815,6 +842,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1416,8 +1444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N9999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1577,7 +1605,7 @@
       <c r="C7" s="37"/>
       <c r="D7" s="40">
         <f>SUM(Tableau1[Durée])</f>
-        <v>0.44374999999999976</v>
+        <v>14.514861111111111</v>
       </c>
       <c r="E7" s="41"/>
       <c r="G7" s="4">
@@ -1976,57 +2004,113 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
+    <row r="21" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G21" s="4">
+        <v>44985</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="J21" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G22" s="4"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G22" s="4">
+        <v>44986</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="I22" s="6">
+        <v>0.61111111111111105</v>
+      </c>
       <c r="J22" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="7"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G23" s="4"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="6"/>
+        <v>2.4305555555555469E-2</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G23" s="4">
+        <v>44986</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="I23" s="6">
+        <v>14.616250000000001</v>
+      </c>
       <c r="J23" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G24" s="4"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
+        <v>14.004444444444445</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G24" s="4">
+        <v>44986</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.6166666666666667</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0.62777777777777777</v>
+      </c>
       <c r="J24" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
+        <v>1.1111111111111072E-2</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G25" s="4"/>
@@ -44433,14 +44517,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="33" customHeight="1" x14ac:dyDescent="0.35">
@@ -44465,9 +44550,15 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="C4" s="52">
+        <v>45009</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C5" s="28"/>

</xml_diff>

<commit_message>
Mise a jour de journal de travail
Mis a jour du journal de travail par rapport a la semaine passé
</commit_message>
<xml_diff>
--- a/Documentation/JournauxMarcosDMS.xlsx
+++ b/Documentation/JournauxMarcosDMS.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>On a codé le lost ainsi que les autres redirections de la page d'acceuil. Ajouter le css. On a codé le gabarit. Modifier l'index.</t>
+  </si>
+  <si>
+    <t>On essaie de débuger le register parce que ça veut pas écrire dans le register.</t>
+  </si>
+  <si>
+    <t>On à codé le login ainsi que le register.</t>
   </si>
 </sst>
 </file>
@@ -792,13 +798,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -824,36 +860,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1460,7 +1466,7 @@
   <dimension ref="B1:N9999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N30" sqref="N29:N30"/>
+      <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,27 +1488,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1510,14 +1516,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="40" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="51"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1544,14 +1550,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="38" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="49"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1579,14 +1585,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="36">
+      <c r="C6" s="40"/>
+      <c r="D6" s="46">
         <v>44957</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="47"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1614,15 +1620,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50">
+      <c r="C7" s="38"/>
+      <c r="D7" s="41">
         <f>SUM(Tableau1[Durée])</f>
-        <v>14.576666666666666</v>
-      </c>
-      <c r="E7" s="51"/>
+        <v>14.673888888888888</v>
+      </c>
+      <c r="E7" s="42"/>
       <c r="G7" s="4">
         <v>44927</v>
       </c>
@@ -1678,10 +1684,10 @@
     </row>
     <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="32"/>
       <c r="G9" s="4">
         <v>44927</v>
       </c>
@@ -1712,10 +1718,10 @@
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="45"/>
+      <c r="D10" s="34"/>
       <c r="G10" s="4">
         <v>44927</v>
       </c>
@@ -1746,10 +1752,10 @@
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="36"/>
       <c r="G11" s="4">
         <v>44927</v>
       </c>
@@ -2182,30 +2188,58 @@
       </c>
     </row>
     <row r="27" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G27" s="4"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="6"/>
+      <c r="G27" s="4">
+        <v>44987</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.5625</v>
+      </c>
+      <c r="I27" s="6">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="J27" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="7"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-    </row>
-    <row r="28" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G28" s="4"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="6"/>
+        <v>6.597222222222221E-2</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G28" s="4">
+        <v>44987</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="I28" s="6">
+        <v>0.70486111111111116</v>
+      </c>
       <c r="J28" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K28" s="7"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="29" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G29" s="4"/>
@@ -44532,18 +44566,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:N2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G1:N2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -44911,12 +44945,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45090,15 +45121,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45122,17 +45164,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mise a jour de mon journal de travail
J'ai mis a jour mon journal de travail.
</commit_message>
<xml_diff>
--- a/Documentation/JournauxMarcosDMS.xlsx
+++ b/Documentation/JournauxMarcosDMS.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="82">
   <si>
     <t>Nom du Projet :</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>Finalisation de la page login (fonctionnable)</t>
+  </si>
+  <si>
+    <t>Création de la fonction logout (complète)</t>
+  </si>
+  <si>
+    <t>Création de la page panier ainsi que la fonction pour rajouter les produits dedans</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -813,13 +822,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -845,36 +884,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1480,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N9999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="E25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,27 +1512,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
     </row>
     <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="F2" s="17"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F3" s="18"/>
@@ -1531,14 +1540,14 @@
       <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:14" ht="65.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="40" t="s">
+      <c r="C4" s="45"/>
+      <c r="D4" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="41"/>
+      <c r="E4" s="51"/>
       <c r="G4" s="20" t="s">
         <v>1</v>
       </c>
@@ -1565,14 +1574,14 @@
       </c>
     </row>
     <row r="5" spans="2:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="38" t="s">
+      <c r="C5" s="40"/>
+      <c r="D5" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="49"/>
       <c r="G5" s="4">
         <v>44957</v>
       </c>
@@ -1600,14 +1609,14 @@
       </c>
     </row>
     <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="36">
+      <c r="C6" s="40"/>
+      <c r="D6" s="46">
         <v>44957</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="47"/>
       <c r="G6" s="4">
         <v>44957</v>
       </c>
@@ -1635,15 +1644,15 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50">
+      <c r="C7" s="38"/>
+      <c r="D7" s="41">
         <f>SUM(Tableau1[Durée])</f>
-        <v>15.12875</v>
-      </c>
-      <c r="E7" s="51"/>
+        <v>15.2225</v>
+      </c>
+      <c r="E7" s="42"/>
       <c r="G7" s="4">
         <v>44927</v>
       </c>
@@ -1699,10 +1708,10 @@
     </row>
     <row r="9" spans="2:14" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16"/>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="43"/>
+      <c r="D9" s="32"/>
       <c r="G9" s="4">
         <v>44927</v>
       </c>
@@ -1733,10 +1742,10 @@
       <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="45"/>
+      <c r="D10" s="34"/>
       <c r="G10" s="4">
         <v>44927</v>
       </c>
@@ -1767,10 +1776,10 @@
       <c r="B11" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="36"/>
       <c r="G11" s="4">
         <v>44927</v>
       </c>
@@ -2473,30 +2482,58 @@
       </c>
     </row>
     <row r="37" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G37" s="4"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="6"/>
+      <c r="G37" s="4">
+        <v>45014</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="I37" s="6">
+        <v>0.62847222222222221</v>
+      </c>
       <c r="J37" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K37" s="7"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G38" s="4"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="6"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="M37" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="7:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G38" s="4">
+        <v>45014</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="I38" s="6">
+        <v>0.70138888888888884</v>
+      </c>
       <c r="J38" s="5">
         <f>Tableau1[[#This Row],[Heure fin]]-Tableau1[[#This Row],[Heure debut]]</f>
-        <v>0</v>
-      </c>
-      <c r="K38" s="7"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
+        <v>6.2499999999999889E-2</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="39" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G39" s="4"/>
@@ -2509,7 +2546,9 @@
       <c r="K39" s="7"/>
       <c r="L39" s="8"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
+      <c r="N39" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="40" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G40" s="4"/>
@@ -44693,18 +44732,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:N2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D4:E4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="G1:N2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D4:E4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1"/>
@@ -45072,12 +45111,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45251,15 +45287,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45283,17 +45330,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D38AEF9-57C3-439A-B892-EB0F14AB4CC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE66B988-21FD-4E82-857E-C2E9A6618F3F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="9b42e094-9454-4e38-a519-f9a276a20d04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>